<commit_message>
Se implemento la funcion que agrupa por semana
</commit_message>
<xml_diff>
--- a/Data/Inputs/datos_combinados.xlsx
+++ b/Data/Inputs/datos_combinados.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,11 @@
           <t>date_pay_settle</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>carpeta_cliente</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -487,21 +492,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11012024 </t>
-        </is>
+      <c r="B2" t="n">
+        <v>11012024</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>ALEJANDRA S FASHIÓON INC</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>35,783.00</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>5293</t>
@@ -510,6 +516,11 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>2024-11-08</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -519,24 +530,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11012024 </t>
-        </is>
+      <c r="B3" t="n">
+        <v>11012024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>ALEJANDRA'S FASHIOÓN, INC.</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>4,438.24</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>2024-11-08</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -546,10 +564,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>11012024</t>
-        </is>
+      <c r="B4" t="n">
+        <v>11012024</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -564,6 +580,15 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>4438.24</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -573,21 +598,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11082024 </t>
-        </is>
+      <c r="B5" t="n">
+        <v>11082024</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>ALEJANDRA S FASHIÓON INC</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>36,233.65</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>5293</t>
@@ -596,6 +622,11 @@
       <c r="I5" t="inlineStr">
         <is>
           <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -605,24 +636,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11082024 </t>
-        </is>
+      <c r="B6" t="n">
+        <v>11082024</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>ALEJANDRA'S FASHIOÓN, INC.</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>4,416.39</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -632,10 +670,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>11082024</t>
-        </is>
+      <c r="B7" t="n">
+        <v>11082024</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -650,6 +686,15 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>4416.39</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -659,21 +704,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11152024  </t>
-        </is>
+      <c r="B8" t="n">
+        <v>11152024</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>ALEJANDRA S FASHIÓON INC</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>38,771.93</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>5293</t>
@@ -682,6 +728,11 @@
       <c r="I8" t="inlineStr">
         <is>
           <t>2024-11-20</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -691,24 +742,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11152024 </t>
-        </is>
+      <c r="B9" t="n">
+        <v>11152024</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>ALEJANDRA'S FASHIOÓN, INC.</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>4,793.73</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>2024-11-20</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -718,10 +776,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11152024</t>
-        </is>
+      <c r="B10" t="n">
+        <v>11152024</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -736,6 +792,15 @@
       <c r="E10" t="inlineStr">
         <is>
           <t>4793.73</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -745,21 +810,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11222024 </t>
-        </is>
+      <c r="B11" t="n">
+        <v>11222024</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>ALEJANDRA S FASHIÓON INC</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
           <t>37,915.74</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>5293</t>
@@ -768,6 +834,11 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>2024-11-27</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -777,24 +848,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11222024 </t>
-        </is>
+      <c r="B12" t="n">
+        <v>11222024</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>ALEJANDRA'S FASHIOÓN, INC.</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
           <t>4,702.90</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>2024-11-27</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -804,10 +882,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>11222024</t>
-        </is>
+      <c r="B13" t="n">
+        <v>11222024</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -822,6 +898,15 @@
       <c r="E13" t="inlineStr">
         <is>
           <t>4702.90</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -831,21 +916,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11292024 </t>
-        </is>
+      <c r="B14" t="n">
+        <v>11292024</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>ALEJANDRA S FASHIÓON INC</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
           <t>41,179.84</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>5293</t>
@@ -854,6 +940,11 @@
       <c r="I14" t="inlineStr">
         <is>
           <t>2024-12-04</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -863,24 +954,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11292024 </t>
-        </is>
+      <c r="B15" t="n">
+        <v>11292024</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>ALEJANDRA'S FASHIOÓN, INC.</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>5,151.26</t>
         </is>
       </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>2024-12-04</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -890,10 +988,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>11292024</t>
-        </is>
+      <c r="B16" t="n">
+        <v>11292024</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -908,6 +1004,15 @@
       <c r="E16" t="inlineStr">
         <is>
           <t>5151.17</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Alejandra</t>
         </is>
       </c>
     </row>
@@ -917,21 +1022,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11012024 </t>
-        </is>
+      <c r="B17" t="n">
+        <v>11012024</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>546.52</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>7888</t>
@@ -940,6 +1046,11 @@
       <c r="I17" t="inlineStr">
         <is>
           <t>2024-11-06</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -949,24 +1060,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11012024 </t>
-        </is>
+      <c r="B18" t="n">
+        <v>11012024</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>AVINA PRODUCE INC</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
           <t>72.92</t>
         </is>
       </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
           <t>2024-11-06</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -976,10 +1094,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>11012024</t>
-        </is>
+      <c r="B19" t="n">
+        <v>11012024</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -994,6 +1110,15 @@
       <c r="E19" t="inlineStr">
         <is>
           <t>72.92</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1003,21 +1128,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11082024 </t>
-        </is>
+      <c r="B20" t="n">
+        <v>11082024</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
           <t>546.52</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>7888</t>
@@ -1026,6 +1152,11 @@
       <c r="I20" t="inlineStr">
         <is>
           <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1035,24 +1166,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11082024 </t>
-        </is>
+      <c r="B21" t="n">
+        <v>11082024</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>AVINA PRODUCE INC</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
           <t>72.92</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
           <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1062,10 +1200,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11082024</t>
-        </is>
+      <c r="B22" t="n">
+        <v>11082024</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1080,6 +1216,15 @@
       <c r="E22" t="inlineStr">
         <is>
           <t>72.92</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1089,21 +1234,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11152024  </t>
-        </is>
+      <c r="B23" t="n">
+        <v>11152024</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
           <t>546.52</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
           <t>7888</t>
@@ -1112,6 +1258,11 @@
       <c r="I23" t="inlineStr">
         <is>
           <t>2024-11-20</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1121,24 +1272,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11152024 </t>
-        </is>
+      <c r="B24" t="n">
+        <v>11152024</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>AVINA PRODUCE INC</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
           <t>72.92</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
           <t>2024-11-20</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1148,10 +1306,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>11152024</t>
-        </is>
+      <c r="B25" t="n">
+        <v>11152024</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1166,6 +1322,15 @@
       <c r="E25" t="inlineStr">
         <is>
           <t>72.92</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1175,21 +1340,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11222024 </t>
-        </is>
+      <c r="B26" t="n">
+        <v>11222024</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>AVINA PRODUCE TIN: xxxxx8949</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>546.52</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
           <t>7888</t>
@@ -1198,6 +1364,11 @@
       <c r="I26" t="inlineStr">
         <is>
           <t>2024-11-27</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1207,24 +1378,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11222024 </t>
-        </is>
+      <c r="B27" t="n">
+        <v>11222024</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>AVINA PRODUCE INC</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>72.92</t>
         </is>
       </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
           <t>2024-11-27</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1234,10 +1412,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>11222024</t>
-        </is>
+      <c r="B28" t="n">
+        <v>11222024</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1252,6 +1428,15 @@
       <c r="E28" t="inlineStr">
         <is>
           <t>72.92</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1261,21 +1446,22 @@
           <t>941</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11292024 </t>
-        </is>
+      <c r="B29" t="n">
+        <v>11292024</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>AVINA PRODUCE</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
           <t>1,426.00</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
           <t>7888</t>
@@ -1284,6 +1470,11 @@
       <c r="I29" t="inlineStr">
         <is>
           <t>2024-12-04</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1293,24 +1484,31 @@
           <t>EDD</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11292024 </t>
-        </is>
+      <c r="B30" t="n">
+        <v>11292024</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>AVINA PRODUCE INC</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
           <t>72.92</t>
         </is>
       </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
           <t>2024-12-04</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1320,10 +1518,8 @@
           <t>general</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>11292024</t>
-        </is>
+      <c r="B31" t="n">
+        <v>11292024</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1338,6 +1534,15 @@
       <c r="E31" t="inlineStr">
         <is>
           <t>72.92</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Avina</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1363,12 +1568,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>tipo_archivo</t>
+          <t>carpeta_cliente</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>fecha_pdf</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1389,29 +1594,17 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>EDD_payment_amount</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>account_number</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>date_pay_settle</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ALEJANDRAS FASHION INC</t>
-        </is>
+          <t>Alejandra</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11012024</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1421,271 +1614,286 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>4438.24</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>35,783.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4,438.24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>941</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>Alejandra</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11082024</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>36233.65</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4416.39</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>35,783.00</t>
+          <t>36,233.65</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4,438.24</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>5293</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2024-11-08</t>
+          <t>4,416.39</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ALEJANDRAS FASHION INC</t>
-        </is>
+          <t>Alejandra</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>11152024</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>36233.65</t>
+          <t>38771.93</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4416.39</t>
+          <t>4793.73</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>38,771.93</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>4,793.73</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>941</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>Alejandra</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11222024</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>37915.74</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4702.90</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>36,233.65</t>
+          <t>37,915.74</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4,416.39</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>5293</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2024-11-13</t>
+          <t>4,702.90</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ALEJANDRAS FASHION INC</t>
-        </is>
+          <t>Alejandra</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>11292024</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>38771.93</t>
+          <t>41179.84</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4793.73</t>
+          <t>5151.17</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>41,179.84</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5,151.26</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EDD</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ALEJANDRA'S FASHIOÓN, INC.</t>
+          <t>Avina</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>11012024</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>546.52</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>72.92</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>546.52</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4,793.73</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2024-11-20</t>
+          <t>72.92</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>941</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>Avina</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>11082024</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>546.52</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>72.92</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>38,771.93</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>5293</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2024-11-20</t>
+          <t>546.52</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>72.92</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ALEJANDRAS FASHION INC</t>
-        </is>
+          <t>Avina</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>11152024</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>37915.74</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4702.90</t>
+          <t>72.92</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>546.52</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>72.92</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>941</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
+          <t>Avina</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>11222024</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>546.52</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>72.92</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>37,915.74</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>4,702.90</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5293</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2024-11-27</t>
+          <t>72.92</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ALEJANDRAS FASHION INC</t>
-        </is>
+          <t>Avina</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>11292024</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>41179.84</t>
+          <t>546.52</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5151.17</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>941</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ALEJANDRA S FASHIÓON INC</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>41,179.84</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>5,151.26</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>5293</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2024-12-04</t>
+          <t>72.92</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1,426.00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>72.92</t>
         </is>
       </c>
     </row>

</xml_diff>